<commit_message>
Map Maker version 2
</commit_message>
<xml_diff>
--- a/MapMaker/MiniMapView.xlsx
+++ b/MapMaker/MiniMapView.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
   <si>
     <t>Max</t>
   </si>
@@ -128,13 +130,37 @@
   </si>
   <si>
     <t>cen</t>
+  </si>
+  <si>
+    <t>Tiles high</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>Display Height</t>
+  </si>
+  <si>
+    <t>Scroll Max</t>
+  </si>
+  <si>
+    <t>Scroll %</t>
+  </si>
+  <si>
+    <t>Grid</t>
+  </si>
+  <si>
+    <t>Final</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +172,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -171,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -196,6 +229,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1661,7 +1698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -1921,4 +1958,291 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="3">
+        <v>459</v>
+      </c>
+      <c r="C3" s="3">
+        <v>361</v>
+      </c>
+      <c r="D3" s="3">
+        <v>10.5</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="10">
+        <f>E3/$B$3</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>160</v>
+      </c>
+      <c r="H3" s="3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E4" s="3">
+        <v>166</v>
+      </c>
+      <c r="F4" s="10">
+        <f>E4/$B$3</f>
+        <v>0.36165577342047928</v>
+      </c>
+      <c r="G4" s="3">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E5" s="3">
+        <v>298</v>
+      </c>
+      <c r="F5" s="10">
+        <f>E5/$B$3</f>
+        <v>0.64923747276688448</v>
+      </c>
+      <c r="G5" s="3">
+        <v>448</v>
+      </c>
+      <c r="H5" s="3">
+        <f>448+32</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E6" s="3">
+        <v>327</v>
+      </c>
+      <c r="F6" s="10">
+        <f t="shared" ref="F6:F8" si="0">E6/$B$3</f>
+        <v>0.71241830065359479</v>
+      </c>
+      <c r="H6" s="3">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E7" s="3">
+        <v>360</v>
+      </c>
+      <c r="F7" s="10">
+        <f t="shared" si="0"/>
+        <v>0.78431372549019607</v>
+      </c>
+      <c r="G7" s="3">
+        <v>512</v>
+      </c>
+      <c r="H7" s="3">
+        <f>512+32</f>
+        <v>544</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E8" s="3">
+        <v>459</v>
+      </c>
+      <c r="F8" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>640</v>
+      </c>
+      <c r="H8" s="3">
+        <v>640</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:H10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="11">
+        <v>32</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>64</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="11">
+        <v>32</v>
+      </c>
+      <c r="D5" s="11">
+        <v>32</v>
+      </c>
+      <c r="G5">
+        <v>64</v>
+      </c>
+      <c r="H5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>32</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="11">
+        <v>32</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>64</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>64</v>
+      </c>
+      <c r="D9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="11">
+        <v>32</v>
+      </c>
+      <c r="D10" s="11">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Map Maker version 3
</commit_message>
<xml_diff>
--- a/MapMaker/MiniMapView.xlsx
+++ b/MapMaker/MiniMapView.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="73">
   <si>
     <t>Max</t>
   </si>
@@ -147,10 +148,106 @@
     <t>Scroll %</t>
   </si>
   <si>
-    <t>Grid</t>
+    <t>Sector</t>
+  </si>
+  <si>
+    <t>Tiles Wide</t>
+  </si>
+  <si>
+    <t>Tiles High</t>
+  </si>
+  <si>
+    <t>Initial</t>
   </si>
   <si>
     <t>Final</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>Move NE</t>
+  </si>
+  <si>
+    <t>Move SE</t>
+  </si>
+  <si>
+    <t>Move NW</t>
+  </si>
+  <si>
+    <t>Move SW</t>
+  </si>
+  <si>
+    <t>Move E</t>
+  </si>
+  <si>
+    <t>Move W</t>
+  </si>
+  <si>
+    <t>Move N</t>
+  </si>
+  <si>
+    <t>Move S</t>
+  </si>
+  <si>
+    <t>Expand E</t>
+  </si>
+  <si>
+    <t>Expand W</t>
+  </si>
+  <si>
+    <t>Expand N</t>
+  </si>
+  <si>
+    <t>Expand S</t>
+  </si>
+  <si>
+    <t>Expand NE</t>
+  </si>
+  <si>
+    <t>Expand NW</t>
+  </si>
+  <si>
+    <t>Expand SE</t>
+  </si>
+  <si>
+    <t>Expand SW</t>
+  </si>
+  <si>
+    <t>Shrink E</t>
+  </si>
+  <si>
+    <t>Shrink W</t>
+  </si>
+  <si>
+    <t>Shrink N</t>
+  </si>
+  <si>
+    <t>Shrink S</t>
+  </si>
+  <si>
+    <t>Shrink NE</t>
+  </si>
+  <si>
+    <t>Shrink NW</t>
+  </si>
+  <si>
+    <t>Shrink SE</t>
+  </si>
+  <si>
+    <t>Shrink SW</t>
   </si>
 </sst>
 </file>
@@ -160,7 +257,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +276,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -204,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -232,7 +335,18 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2101,148 +2215,1851 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H10"/>
+  <dimension ref="B2:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="10" width="9.140625" style="3"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>0</v>
+      <c r="I2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="11">
+        <v>2</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0</v>
+      </c>
+      <c r="E3" s="11">
+        <v>0</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0</v>
+      </c>
+      <c r="G3" s="11">
+        <v>352</v>
+      </c>
+      <c r="H3" s="11">
+        <f>G3/32</f>
+        <v>11</v>
+      </c>
+      <c r="I3" s="11">
+        <v>160</v>
+      </c>
+      <c r="J3" s="11">
+        <f>I3/32</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="11">
+        <v>3</v>
       </c>
       <c r="C4" s="11">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="D4" s="11">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>64</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>0</v>
+        <f>11*32</f>
+        <v>352</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0</v>
+      </c>
+      <c r="G4" s="11">
+        <v>640</v>
+      </c>
+      <c r="H4" s="11">
+        <f t="shared" ref="H4:H6" si="0">G4/32</f>
+        <v>20</v>
+      </c>
+      <c r="I4" s="11">
+        <v>320</v>
+      </c>
+      <c r="J4" s="11">
+        <f t="shared" ref="J4:J6" si="1">I4/32</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="11">
+        <v>1</v>
       </c>
       <c r="C5" s="11">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="D5" s="11">
-        <v>32</v>
-      </c>
-      <c r="G5">
-        <v>64</v>
-      </c>
-      <c r="H5">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>32</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="11">
-        <v>32</v>
-      </c>
-      <c r="D7" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>64</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>64</v>
-      </c>
-      <c r="D9">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" s="11">
-        <v>32</v>
-      </c>
-      <c r="D10" s="11">
-        <v>32</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E5" s="11">
+        <v>0</v>
+      </c>
+      <c r="F5" s="11">
+        <f>5*32</f>
+        <v>160</v>
+      </c>
+      <c r="G5" s="11">
+        <v>352</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="I5" s="11">
+        <v>320</v>
+      </c>
+      <c r="J5" s="11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="11">
+        <v>0</v>
+      </c>
+      <c r="C6" s="11">
+        <v>0</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0</v>
+      </c>
+      <c r="F6" s="11">
+        <v>320</v>
+      </c>
+      <c r="G6" s="11">
+        <v>640</v>
+      </c>
+      <c r="H6" s="11">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I6" s="11">
+        <v>800</v>
+      </c>
+      <c r="J6" s="11">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:AE29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" customWidth="1"/>
+    <col min="8" max="9" width="3" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.7109375" style="3" customWidth="1"/>
+    <col min="13" max="14" width="3" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.7109375" style="3" customWidth="1"/>
+    <col min="18" max="19" width="3" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.7109375" style="3" customWidth="1"/>
+    <col min="23" max="24" width="3" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="9.140625" style="3"/>
+    <col min="27" max="27" width="3.7109375" style="3" customWidth="1"/>
+    <col min="28" max="29" width="3" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC2" s="14"/>
+      <c r="AD2" s="14"/>
+      <c r="AE2" s="14"/>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="U3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="V3" s="13"/>
+      <c r="W3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="X3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA3" s="13"/>
+      <c r="AB3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE3" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="3">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3">
+        <v>25</v>
+      </c>
+      <c r="F4" s="3">
+        <v>20</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3">
+        <v>10</v>
+      </c>
+      <c r="J4" s="3">
+        <v>25</v>
+      </c>
+      <c r="K4" s="3">
+        <v>20</v>
+      </c>
+      <c r="M4" s="3">
+        <f>$C4</f>
+        <v>10</v>
+      </c>
+      <c r="N4" s="3">
+        <f>$D4</f>
+        <v>10</v>
+      </c>
+      <c r="O4" s="3">
+        <f>$H4-$C4</f>
+        <v>2</v>
+      </c>
+      <c r="P4" s="3">
+        <f>$F4</f>
+        <v>20</v>
+      </c>
+      <c r="W4" s="3">
+        <f>$M4+$E4</f>
+        <v>35</v>
+      </c>
+      <c r="X4" s="3">
+        <f>$D4</f>
+        <v>10</v>
+      </c>
+      <c r="Y4" s="3">
+        <f>$H4-$C4</f>
+        <v>2</v>
+      </c>
+      <c r="Z4" s="3">
+        <f>$F4</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="3">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3">
+        <v>25</v>
+      </c>
+      <c r="F5" s="3">
+        <v>20</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3">
+        <v>8</v>
+      </c>
+      <c r="I5" s="3">
+        <v>10</v>
+      </c>
+      <c r="J5" s="3">
+        <v>25</v>
+      </c>
+      <c r="K5" s="3">
+        <v>20</v>
+      </c>
+      <c r="M5" s="3">
+        <f>$H5</f>
+        <v>8</v>
+      </c>
+      <c r="N5" s="3">
+        <f>$D5</f>
+        <v>10</v>
+      </c>
+      <c r="O5" s="3">
+        <f>$C5-$H5</f>
+        <v>2</v>
+      </c>
+      <c r="P5" s="3">
+        <f>$F5</f>
+        <v>20</v>
+      </c>
+      <c r="W5" s="3">
+        <f>$H5+$E5</f>
+        <v>33</v>
+      </c>
+      <c r="X5" s="3">
+        <f>$D5</f>
+        <v>10</v>
+      </c>
+      <c r="Y5" s="3">
+        <f>$C5-$H5</f>
+        <v>2</v>
+      </c>
+      <c r="Z5" s="3">
+        <f>$F5</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="3">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3">
+        <v>25</v>
+      </c>
+      <c r="F6" s="3">
+        <v>20</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3">
+        <v>10</v>
+      </c>
+      <c r="I6" s="3">
+        <v>8</v>
+      </c>
+      <c r="J6" s="3">
+        <v>25</v>
+      </c>
+      <c r="K6" s="3">
+        <v>20</v>
+      </c>
+      <c r="R6" s="3">
+        <f>$H6</f>
+        <v>10</v>
+      </c>
+      <c r="S6" s="3">
+        <f>$I6</f>
+        <v>8</v>
+      </c>
+      <c r="T6" s="3">
+        <f>$E6</f>
+        <v>25</v>
+      </c>
+      <c r="U6" s="3">
+        <f>ABS($D6-$I6)</f>
+        <v>2</v>
+      </c>
+      <c r="AB6" s="3">
+        <f>$C6</f>
+        <v>10</v>
+      </c>
+      <c r="AC6" s="3">
+        <f>$I6+$F6</f>
+        <v>28</v>
+      </c>
+      <c r="AD6" s="3">
+        <f>$E6</f>
+        <v>25</v>
+      </c>
+      <c r="AE6" s="3">
+        <f>ABS($D6-$I6)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="3">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3">
+        <v>25</v>
+      </c>
+      <c r="F7" s="3">
+        <v>20</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3">
+        <v>10</v>
+      </c>
+      <c r="I7" s="3">
+        <v>12</v>
+      </c>
+      <c r="J7" s="3">
+        <v>25</v>
+      </c>
+      <c r="K7" s="3">
+        <v>20</v>
+      </c>
+      <c r="R7" s="3">
+        <f>$H7</f>
+        <v>10</v>
+      </c>
+      <c r="S7" s="3">
+        <f>$I7</f>
+        <v>12</v>
+      </c>
+      <c r="T7" s="3">
+        <f>$E7</f>
+        <v>25</v>
+      </c>
+      <c r="U7" s="3">
+        <f t="shared" ref="U7:U11" si="0">ABS($D7-$I7)</f>
+        <v>2</v>
+      </c>
+      <c r="AB7" s="3">
+        <f>$C7</f>
+        <v>10</v>
+      </c>
+      <c r="AC7" s="3">
+        <f>$I7+$F7</f>
+        <v>32</v>
+      </c>
+      <c r="AD7" s="3">
+        <f>$E7</f>
+        <v>25</v>
+      </c>
+      <c r="AE7" s="3">
+        <f t="shared" ref="AE7:AE11" si="1">ABS($D7-$I7)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="3">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3">
+        <v>25</v>
+      </c>
+      <c r="F8" s="3">
+        <v>20</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3">
+        <v>12</v>
+      </c>
+      <c r="I8" s="3">
+        <v>8</v>
+      </c>
+      <c r="J8" s="3">
+        <v>25</v>
+      </c>
+      <c r="K8" s="3">
+        <v>20</v>
+      </c>
+      <c r="M8" s="3">
+        <f>$C8</f>
+        <v>10</v>
+      </c>
+      <c r="N8" s="3">
+        <f>$D8</f>
+        <v>10</v>
+      </c>
+      <c r="O8" s="3">
+        <f>$H8-$C8</f>
+        <v>2</v>
+      </c>
+      <c r="P8" s="3">
+        <f>$F8</f>
+        <v>20</v>
+      </c>
+      <c r="R8" s="3">
+        <f>$H8</f>
+        <v>12</v>
+      </c>
+      <c r="S8" s="3">
+        <f>$I8</f>
+        <v>8</v>
+      </c>
+      <c r="T8" s="3">
+        <f>$E8-($H8-$C8)</f>
+        <v>23</v>
+      </c>
+      <c r="U8" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="W8" s="3">
+        <f>$C8+$E8</f>
+        <v>35</v>
+      </c>
+      <c r="X8" s="3">
+        <f>$I8</f>
+        <v>8</v>
+      </c>
+      <c r="Y8" s="3">
+        <f>$H8-$C8</f>
+        <v>2</v>
+      </c>
+      <c r="Z8" s="3">
+        <f>$F8</f>
+        <v>20</v>
+      </c>
+      <c r="AB8" s="3">
+        <f>$H8</f>
+        <v>12</v>
+      </c>
+      <c r="AC8" s="3">
+        <f>$I8+$F8</f>
+        <v>28</v>
+      </c>
+      <c r="AD8" s="3">
+        <f>$E8-($H8-$C8)</f>
+        <v>23</v>
+      </c>
+      <c r="AE8" s="3">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="3">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3">
+        <v>25</v>
+      </c>
+      <c r="F9" s="3">
+        <v>20</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3">
+        <v>12</v>
+      </c>
+      <c r="I9" s="3">
+        <v>12</v>
+      </c>
+      <c r="J9" s="3">
+        <v>25</v>
+      </c>
+      <c r="K9" s="3">
+        <v>20</v>
+      </c>
+      <c r="M9" s="3">
+        <f>$C9</f>
+        <v>10</v>
+      </c>
+      <c r="N9" s="3">
+        <f>$D9</f>
+        <v>10</v>
+      </c>
+      <c r="O9" s="3">
+        <f>$H9-$C9</f>
+        <v>2</v>
+      </c>
+      <c r="P9" s="3">
+        <f>$F9</f>
+        <v>20</v>
+      </c>
+      <c r="R9" s="3">
+        <f>$H9</f>
+        <v>12</v>
+      </c>
+      <c r="S9" s="3">
+        <f>$D9</f>
+        <v>10</v>
+      </c>
+      <c r="T9" s="3">
+        <f>$E9-($H9-$C9)</f>
+        <v>23</v>
+      </c>
+      <c r="U9" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="W9" s="3">
+        <f>$C9+$E9</f>
+        <v>35</v>
+      </c>
+      <c r="X9" s="3">
+        <f>$I9</f>
+        <v>12</v>
+      </c>
+      <c r="Y9" s="3">
+        <f>$H9-$C9</f>
+        <v>2</v>
+      </c>
+      <c r="Z9" s="3">
+        <f>$F9</f>
+        <v>20</v>
+      </c>
+      <c r="AB9" s="3">
+        <f>$H9</f>
+        <v>12</v>
+      </c>
+      <c r="AC9" s="3">
+        <f>$D9+$F9</f>
+        <v>30</v>
+      </c>
+      <c r="AD9" s="3">
+        <f>$E9-($H9-$C9)</f>
+        <v>23</v>
+      </c>
+      <c r="AE9" s="3">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="3">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3">
+        <v>10</v>
+      </c>
+      <c r="E10" s="3">
+        <v>25</v>
+      </c>
+      <c r="F10" s="3">
+        <v>20</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3">
+        <v>8</v>
+      </c>
+      <c r="I10" s="3">
+        <v>8</v>
+      </c>
+      <c r="J10" s="3">
+        <v>25</v>
+      </c>
+      <c r="K10" s="3">
+        <v>20</v>
+      </c>
+      <c r="M10" s="3">
+        <f>$H10</f>
+        <v>8</v>
+      </c>
+      <c r="N10" s="3">
+        <f>$I10</f>
+        <v>8</v>
+      </c>
+      <c r="O10" s="3">
+        <f>$C10-$H10</f>
+        <v>2</v>
+      </c>
+      <c r="P10" s="3">
+        <f>$F10</f>
+        <v>20</v>
+      </c>
+      <c r="R10" s="3">
+        <f>$C10</f>
+        <v>10</v>
+      </c>
+      <c r="S10" s="3">
+        <f>$I10</f>
+        <v>8</v>
+      </c>
+      <c r="T10" s="3">
+        <f>$E10-($C10-$H10)</f>
+        <v>23</v>
+      </c>
+      <c r="U10" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="W10" s="3">
+        <f>$H10+$E10</f>
+        <v>33</v>
+      </c>
+      <c r="X10" s="3">
+        <f>$D10</f>
+        <v>10</v>
+      </c>
+      <c r="Y10" s="3">
+        <f>$C10-$H10</f>
+        <v>2</v>
+      </c>
+      <c r="Z10" s="3">
+        <f>$F10</f>
+        <v>20</v>
+      </c>
+      <c r="AB10" s="3">
+        <f>$C10</f>
+        <v>10</v>
+      </c>
+      <c r="AC10" s="3">
+        <f>$I10+$F10</f>
+        <v>28</v>
+      </c>
+      <c r="AD10" s="3">
+        <f>$E10-($C10-$H10)</f>
+        <v>23</v>
+      </c>
+      <c r="AE10" s="3">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="3">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3">
+        <v>10</v>
+      </c>
+      <c r="E11" s="3">
+        <v>25</v>
+      </c>
+      <c r="F11" s="3">
+        <v>20</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3">
+        <v>8</v>
+      </c>
+      <c r="I11" s="3">
+        <v>12</v>
+      </c>
+      <c r="J11" s="3">
+        <v>25</v>
+      </c>
+      <c r="K11" s="3">
+        <v>20</v>
+      </c>
+      <c r="M11" s="3">
+        <f>$H11</f>
+        <v>8</v>
+      </c>
+      <c r="N11" s="3">
+        <f>$I11</f>
+        <v>12</v>
+      </c>
+      <c r="O11" s="3">
+        <f>$C11-$H11</f>
+        <v>2</v>
+      </c>
+      <c r="P11" s="3">
+        <f>$F11</f>
+        <v>20</v>
+      </c>
+      <c r="R11" s="3">
+        <f>$C11</f>
+        <v>10</v>
+      </c>
+      <c r="S11" s="3">
+        <f>$D11</f>
+        <v>10</v>
+      </c>
+      <c r="T11" s="3">
+        <f>$E11-($C11-$H11)</f>
+        <v>23</v>
+      </c>
+      <c r="U11" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="W11" s="3">
+        <f>$H11+$E11</f>
+        <v>33</v>
+      </c>
+      <c r="X11" s="3">
+        <f>$D11</f>
+        <v>10</v>
+      </c>
+      <c r="Y11" s="3">
+        <f>$C11-$H11</f>
+        <v>2</v>
+      </c>
+      <c r="Z11" s="3">
+        <f>$F11</f>
+        <v>20</v>
+      </c>
+      <c r="AB11" s="3">
+        <f>$C11</f>
+        <v>10</v>
+      </c>
+      <c r="AC11" s="3">
+        <f>$D11+$F11</f>
+        <v>30</v>
+      </c>
+      <c r="AD11" s="3">
+        <f>$E11-($C11-$H11)</f>
+        <v>23</v>
+      </c>
+      <c r="AE11" s="3">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="3">
+        <v>10</v>
+      </c>
+      <c r="D13" s="3">
+        <v>10</v>
+      </c>
+      <c r="E13" s="3">
+        <v>25</v>
+      </c>
+      <c r="F13" s="3">
+        <v>20</v>
+      </c>
+      <c r="H13" s="3">
+        <v>10</v>
+      </c>
+      <c r="I13" s="3">
+        <v>8</v>
+      </c>
+      <c r="J13" s="3">
+        <v>25</v>
+      </c>
+      <c r="K13" s="3">
+        <v>22</v>
+      </c>
+      <c r="R13" s="3">
+        <f>$H13</f>
+        <v>10</v>
+      </c>
+      <c r="S13" s="3">
+        <f>$I13</f>
+        <v>8</v>
+      </c>
+      <c r="T13" s="3">
+        <f>$J13</f>
+        <v>25</v>
+      </c>
+      <c r="U13" s="3">
+        <f>$K13-$F13</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="3">
+        <v>10</v>
+      </c>
+      <c r="D14" s="3">
+        <v>10</v>
+      </c>
+      <c r="E14" s="3">
+        <v>25</v>
+      </c>
+      <c r="F14" s="3">
+        <v>20</v>
+      </c>
+      <c r="H14" s="3">
+        <v>10</v>
+      </c>
+      <c r="I14" s="3">
+        <v>10</v>
+      </c>
+      <c r="J14" s="3">
+        <v>25</v>
+      </c>
+      <c r="K14" s="3">
+        <v>22</v>
+      </c>
+      <c r="AB14" s="3">
+        <f>$H14</f>
+        <v>10</v>
+      </c>
+      <c r="AC14" s="3">
+        <f>$D14+$F14</f>
+        <v>30</v>
+      </c>
+      <c r="AD14" s="3">
+        <f>$J14</f>
+        <v>25</v>
+      </c>
+      <c r="AE14" s="3">
+        <f>$K14-$F14</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="3">
+        <v>10</v>
+      </c>
+      <c r="D15" s="3">
+        <v>10</v>
+      </c>
+      <c r="E15" s="3">
+        <v>25</v>
+      </c>
+      <c r="F15" s="3">
+        <v>20</v>
+      </c>
+      <c r="H15" s="3">
+        <v>10</v>
+      </c>
+      <c r="I15" s="3">
+        <v>10</v>
+      </c>
+      <c r="J15" s="3">
+        <v>27</v>
+      </c>
+      <c r="K15" s="3">
+        <v>20</v>
+      </c>
+      <c r="W15" s="3">
+        <f>$C15+$E15</f>
+        <v>35</v>
+      </c>
+      <c r="X15" s="3">
+        <f>$I15</f>
+        <v>10</v>
+      </c>
+      <c r="Y15" s="3">
+        <f>$J15-$E15</f>
+        <v>2</v>
+      </c>
+      <c r="Z15" s="3">
+        <f>$K15</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="3">
+        <v>10</v>
+      </c>
+      <c r="D16" s="3">
+        <v>10</v>
+      </c>
+      <c r="E16" s="3">
+        <v>25</v>
+      </c>
+      <c r="F16" s="3">
+        <v>20</v>
+      </c>
+      <c r="H16" s="3">
+        <v>8</v>
+      </c>
+      <c r="I16" s="3">
+        <v>10</v>
+      </c>
+      <c r="J16" s="3">
+        <v>27</v>
+      </c>
+      <c r="K16" s="3">
+        <v>20</v>
+      </c>
+      <c r="M16" s="3">
+        <f>$H16</f>
+        <v>8</v>
+      </c>
+      <c r="N16" s="3">
+        <f>$I16</f>
+        <v>10</v>
+      </c>
+      <c r="O16" s="3">
+        <f>$J16-$E16</f>
+        <v>2</v>
+      </c>
+      <c r="P16" s="3">
+        <f>$K16</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="3">
+        <v>10</v>
+      </c>
+      <c r="D17" s="3">
+        <v>10</v>
+      </c>
+      <c r="E17" s="3">
+        <v>25</v>
+      </c>
+      <c r="F17" s="3">
+        <v>20</v>
+      </c>
+      <c r="H17" s="3">
+        <v>10</v>
+      </c>
+      <c r="I17" s="3">
+        <v>8</v>
+      </c>
+      <c r="J17" s="3">
+        <v>27</v>
+      </c>
+      <c r="K17" s="3">
+        <v>22</v>
+      </c>
+      <c r="R17" s="3">
+        <f>$H17</f>
+        <v>10</v>
+      </c>
+      <c r="S17" s="3">
+        <f>$I17</f>
+        <v>8</v>
+      </c>
+      <c r="T17" s="3">
+        <f>$J17</f>
+        <v>27</v>
+      </c>
+      <c r="U17" s="3">
+        <f>$K17-$F17</f>
+        <v>2</v>
+      </c>
+      <c r="W17" s="3">
+        <f>$C17+$E17</f>
+        <v>35</v>
+      </c>
+      <c r="X17" s="3">
+        <f>$I17</f>
+        <v>8</v>
+      </c>
+      <c r="Y17" s="3">
+        <f>$J17-$E17</f>
+        <v>2</v>
+      </c>
+      <c r="Z17" s="3">
+        <f>$K17</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="3">
+        <v>10</v>
+      </c>
+      <c r="D18" s="3">
+        <v>10</v>
+      </c>
+      <c r="E18" s="3">
+        <v>25</v>
+      </c>
+      <c r="F18" s="3">
+        <v>20</v>
+      </c>
+      <c r="H18" s="3">
+        <v>8</v>
+      </c>
+      <c r="I18" s="3">
+        <v>8</v>
+      </c>
+      <c r="J18" s="3">
+        <v>27</v>
+      </c>
+      <c r="K18" s="3">
+        <v>22</v>
+      </c>
+      <c r="M18" s="3">
+        <f>$H18</f>
+        <v>8</v>
+      </c>
+      <c r="N18" s="3">
+        <f>$I18</f>
+        <v>8</v>
+      </c>
+      <c r="O18" s="3">
+        <f>$J18-$E18</f>
+        <v>2</v>
+      </c>
+      <c r="P18" s="3">
+        <f>$K18</f>
+        <v>22</v>
+      </c>
+      <c r="R18" s="3">
+        <f>$C18</f>
+        <v>10</v>
+      </c>
+      <c r="S18" s="3">
+        <f>$I18</f>
+        <v>8</v>
+      </c>
+      <c r="T18" s="3">
+        <f>$E18-($J18-$E18)</f>
+        <v>23</v>
+      </c>
+      <c r="U18" s="3">
+        <f>$K18-$F18</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="3">
+        <v>10</v>
+      </c>
+      <c r="D19" s="3">
+        <v>10</v>
+      </c>
+      <c r="E19" s="3">
+        <v>25</v>
+      </c>
+      <c r="F19" s="3">
+        <v>20</v>
+      </c>
+      <c r="H19" s="3">
+        <v>10</v>
+      </c>
+      <c r="I19" s="3">
+        <v>10</v>
+      </c>
+      <c r="J19" s="3">
+        <v>27</v>
+      </c>
+      <c r="K19" s="3">
+        <v>22</v>
+      </c>
+      <c r="W19" s="3">
+        <f>$C19+E19</f>
+        <v>35</v>
+      </c>
+      <c r="X19" s="3">
+        <f>$D19</f>
+        <v>10</v>
+      </c>
+      <c r="Y19" s="3">
+        <f>$J19 - $E19</f>
+        <v>2</v>
+      </c>
+      <c r="Z19" s="3">
+        <f>$K19</f>
+        <v>22</v>
+      </c>
+      <c r="AB19" s="3">
+        <f>C19</f>
+        <v>10</v>
+      </c>
+      <c r="AC19" s="3">
+        <f>$D19+$F19</f>
+        <v>30</v>
+      </c>
+      <c r="AD19" s="3">
+        <f>$E19</f>
+        <v>25</v>
+      </c>
+      <c r="AE19" s="3">
+        <f>$K19-$F19</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="3">
+        <v>10</v>
+      </c>
+      <c r="D20" s="3">
+        <v>10</v>
+      </c>
+      <c r="E20" s="3">
+        <v>25</v>
+      </c>
+      <c r="F20" s="3">
+        <v>20</v>
+      </c>
+      <c r="H20" s="3">
+        <v>8</v>
+      </c>
+      <c r="I20" s="3">
+        <v>10</v>
+      </c>
+      <c r="J20" s="3">
+        <v>27</v>
+      </c>
+      <c r="K20" s="3">
+        <v>22</v>
+      </c>
+      <c r="M20" s="3">
+        <f>$H20</f>
+        <v>8</v>
+      </c>
+      <c r="N20" s="3">
+        <f>$I20</f>
+        <v>10</v>
+      </c>
+      <c r="O20" s="3">
+        <f>$J20-$E20</f>
+        <v>2</v>
+      </c>
+      <c r="P20" s="3">
+        <f>$K20</f>
+        <v>22</v>
+      </c>
+      <c r="AB20" s="3">
+        <f>C20</f>
+        <v>10</v>
+      </c>
+      <c r="AC20" s="3">
+        <f>$D20+$F20</f>
+        <v>30</v>
+      </c>
+      <c r="AD20" s="3">
+        <f>$E20</f>
+        <v>25</v>
+      </c>
+      <c r="AE20" s="3">
+        <f>$K20-$F20</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="3">
+        <v>10</v>
+      </c>
+      <c r="D22" s="3">
+        <v>10</v>
+      </c>
+      <c r="E22" s="3">
+        <v>25</v>
+      </c>
+      <c r="F22" s="3">
+        <v>20</v>
+      </c>
+      <c r="H22" s="3">
+        <v>10</v>
+      </c>
+      <c r="I22" s="3">
+        <v>8</v>
+      </c>
+      <c r="J22" s="3">
+        <v>25</v>
+      </c>
+      <c r="K22" s="3">
+        <v>18</v>
+      </c>
+      <c r="R22" s="3">
+        <f>$C22</f>
+        <v>10</v>
+      </c>
+      <c r="S22" s="3">
+        <f>$I22</f>
+        <v>8</v>
+      </c>
+      <c r="T22" s="3">
+        <f>$E22-($J22-$E22)</f>
+        <v>25</v>
+      </c>
+      <c r="U22" s="3">
+        <f>$F22-$K22</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="3">
+        <v>10</v>
+      </c>
+      <c r="D23" s="3">
+        <v>10</v>
+      </c>
+      <c r="E23" s="3">
+        <v>25</v>
+      </c>
+      <c r="F23" s="3">
+        <v>20</v>
+      </c>
+      <c r="H23" s="3">
+        <v>10</v>
+      </c>
+      <c r="I23" s="3">
+        <v>10</v>
+      </c>
+      <c r="J23" s="3">
+        <v>25</v>
+      </c>
+      <c r="K23" s="3">
+        <v>18</v>
+      </c>
+      <c r="AB23" s="3">
+        <f>$C23</f>
+        <v>10</v>
+      </c>
+      <c r="AC23" s="3">
+        <f>$C23+$K23</f>
+        <v>28</v>
+      </c>
+      <c r="AD23" s="3">
+        <f>$E23</f>
+        <v>25</v>
+      </c>
+      <c r="AE23" s="3">
+        <f>$F23-$K23</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="3">
+        <v>10</v>
+      </c>
+      <c r="D24" s="3">
+        <v>10</v>
+      </c>
+      <c r="E24" s="3">
+        <v>25</v>
+      </c>
+      <c r="F24" s="3">
+        <v>20</v>
+      </c>
+      <c r="H24" s="3">
+        <v>10</v>
+      </c>
+      <c r="I24" s="3">
+        <v>10</v>
+      </c>
+      <c r="J24" s="3">
+        <v>23</v>
+      </c>
+      <c r="K24" s="3">
+        <v>20</v>
+      </c>
+      <c r="W24" s="3">
+        <f>$H24</f>
+        <v>10</v>
+      </c>
+      <c r="X24" s="3">
+        <f>$I24</f>
+        <v>10</v>
+      </c>
+      <c r="Y24" s="3">
+        <f>$E24-$J24</f>
+        <v>2</v>
+      </c>
+      <c r="Z24" s="3">
+        <f>$F24</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="3">
+        <v>10</v>
+      </c>
+      <c r="D25" s="3">
+        <v>10</v>
+      </c>
+      <c r="E25" s="3">
+        <v>25</v>
+      </c>
+      <c r="F25" s="3">
+        <v>20</v>
+      </c>
+      <c r="H25" s="3">
+        <v>12</v>
+      </c>
+      <c r="I25" s="3">
+        <v>10</v>
+      </c>
+      <c r="J25" s="3">
+        <v>23</v>
+      </c>
+      <c r="K25" s="3">
+        <v>20</v>
+      </c>
+      <c r="M25" s="3">
+        <f>$H25</f>
+        <v>12</v>
+      </c>
+      <c r="N25" s="3">
+        <f>$I25</f>
+        <v>10</v>
+      </c>
+      <c r="O25" s="3">
+        <f>$E25-$J25</f>
+        <v>2</v>
+      </c>
+      <c r="P25" s="3">
+        <f>$F25</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="3">
+        <v>10</v>
+      </c>
+      <c r="D26" s="3">
+        <v>10</v>
+      </c>
+      <c r="E26" s="3">
+        <v>25</v>
+      </c>
+      <c r="F26" s="3">
+        <v>20</v>
+      </c>
+      <c r="H26" s="3">
+        <v>10</v>
+      </c>
+      <c r="I26" s="3">
+        <v>12</v>
+      </c>
+      <c r="J26" s="3">
+        <v>23</v>
+      </c>
+      <c r="K26" s="3">
+        <v>18</v>
+      </c>
+      <c r="R26" s="3">
+        <f>$H26</f>
+        <v>10</v>
+      </c>
+      <c r="S26" s="3">
+        <f>$D26</f>
+        <v>10</v>
+      </c>
+      <c r="T26" s="3">
+        <f>$J26</f>
+        <v>23</v>
+      </c>
+      <c r="U26" s="3">
+        <f>$F26-$K26</f>
+        <v>2</v>
+      </c>
+      <c r="W26" s="3">
+        <f>$C26+$J26</f>
+        <v>33</v>
+      </c>
+      <c r="X26" s="3">
+        <f>$D26</f>
+        <v>10</v>
+      </c>
+      <c r="Y26" s="3">
+        <f>$E26-$J26</f>
+        <v>2</v>
+      </c>
+      <c r="Z26" s="3">
+        <f>$F26</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="3">
+        <v>10</v>
+      </c>
+      <c r="D27" s="3">
+        <v>10</v>
+      </c>
+      <c r="E27" s="3">
+        <v>25</v>
+      </c>
+      <c r="F27" s="3">
+        <v>20</v>
+      </c>
+      <c r="H27" s="3">
+        <v>12</v>
+      </c>
+      <c r="I27" s="3">
+        <v>12</v>
+      </c>
+      <c r="J27" s="3">
+        <v>23</v>
+      </c>
+      <c r="K27" s="3">
+        <v>18</v>
+      </c>
+      <c r="M27" s="3">
+        <f>$C27</f>
+        <v>10</v>
+      </c>
+      <c r="N27" s="3">
+        <f>$D27</f>
+        <v>10</v>
+      </c>
+      <c r="O27" s="3">
+        <f>$E27-$J27</f>
+        <v>2</v>
+      </c>
+      <c r="P27" s="3">
+        <f>$F27</f>
+        <v>20</v>
+      </c>
+      <c r="R27" s="3">
+        <f>$H27</f>
+        <v>12</v>
+      </c>
+      <c r="S27" s="3">
+        <f>$D27</f>
+        <v>10</v>
+      </c>
+      <c r="T27" s="3">
+        <f>$J27</f>
+        <v>23</v>
+      </c>
+      <c r="U27" s="3">
+        <f>$F27-$K27</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="3">
+        <v>10</v>
+      </c>
+      <c r="D28" s="3">
+        <v>10</v>
+      </c>
+      <c r="E28" s="3">
+        <v>25</v>
+      </c>
+      <c r="F28" s="3">
+        <v>20</v>
+      </c>
+      <c r="H28" s="3">
+        <v>10</v>
+      </c>
+      <c r="I28" s="3">
+        <v>10</v>
+      </c>
+      <c r="J28" s="3">
+        <v>23</v>
+      </c>
+      <c r="K28" s="3">
+        <v>18</v>
+      </c>
+      <c r="W28" s="3">
+        <f>$C28+$J28</f>
+        <v>33</v>
+      </c>
+      <c r="X28" s="3">
+        <f>$I28</f>
+        <v>10</v>
+      </c>
+      <c r="Y28" s="3">
+        <f>$E28-$J28</f>
+        <v>2</v>
+      </c>
+      <c r="Z28" s="3">
+        <f>$F28</f>
+        <v>20</v>
+      </c>
+      <c r="AB28" s="3">
+        <f>$H28</f>
+        <v>10</v>
+      </c>
+      <c r="AC28" s="3">
+        <f>$I28+$K28</f>
+        <v>28</v>
+      </c>
+      <c r="AD28" s="3">
+        <f>$J28</f>
+        <v>23</v>
+      </c>
+      <c r="AE28" s="3">
+        <f>$F28-$K28</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="3">
+        <v>10</v>
+      </c>
+      <c r="D29" s="3">
+        <v>10</v>
+      </c>
+      <c r="E29" s="3">
+        <v>25</v>
+      </c>
+      <c r="F29" s="3">
+        <v>20</v>
+      </c>
+      <c r="H29" s="3">
+        <v>12</v>
+      </c>
+      <c r="I29" s="3">
+        <v>10</v>
+      </c>
+      <c r="J29" s="3">
+        <v>23</v>
+      </c>
+      <c r="K29" s="3">
+        <v>18</v>
+      </c>
+      <c r="M29" s="3">
+        <f>$C29</f>
+        <v>10</v>
+      </c>
+      <c r="N29" s="3">
+        <f>$I29</f>
+        <v>10</v>
+      </c>
+      <c r="O29" s="3">
+        <f>$E29-$J29</f>
+        <v>2</v>
+      </c>
+      <c r="P29" s="3">
+        <f>$F29</f>
+        <v>20</v>
+      </c>
+      <c r="AB29" s="3">
+        <f>$H29</f>
+        <v>12</v>
+      </c>
+      <c r="AC29" s="3">
+        <f>$I29+$K29</f>
+        <v>28</v>
+      </c>
+      <c r="AD29" s="3">
+        <f>$J29</f>
+        <v>23</v>
+      </c>
+      <c r="AE29" s="3">
+        <f>$F29-$K29</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="AB2:AE2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>